<commit_message>
Mi avance de automation
</commit_message>
<xml_diff>
--- a/Shared.Data/Config.xlsx
+++ b/Shared.Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge.limon\Google Drive\Trabajo\Definity First\Project.Automation\Shared.Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo.castro\Desktop\Project.Automation-master\Shared.Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Browser</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>https://shmqa.definityfirst.com/</t>
-  </si>
-  <si>
     <t>proeza1</t>
   </si>
   <si>
@@ -63,7 +60,7 @@
     <t>VIP User</t>
   </si>
   <si>
-    <t>Firefox</t>
+    <t>https://hl.com</t>
   </si>
 </sst>
 </file>
@@ -517,7 +514,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,21 +539,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="A3" s="12"/>
+      <c r="B3" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{410BCA8B-5562-4FBF-BFE5-9660C712E2DC}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{46645EDB-420B-4361-90C2-7B7459083098}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -587,24 +579,24 @@
     </row>
     <row r="2" spans="1:3" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>